<commit_message>
edits to TM, 1st draft of VM
</commit_message>
<xml_diff>
--- a/Threat-Management-Levels.xlsx
+++ b/Threat-Management-Levels.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="411">
   <si>
     <t>ASVS Item #</t>
   </si>
@@ -1251,6 +1251,18 @@
   </si>
   <si>
     <t>Verify RBAC standard exists</t>
+  </si>
+  <si>
+    <t>Verify critical service classification standard exists</t>
+  </si>
+  <si>
+    <t>Verify asset mapping to critical services standard exists</t>
+  </si>
+  <si>
+    <t>Verify executive buy-in to ensure all relevant business units are to participate</t>
+  </si>
+  <si>
+    <t>Verify ticketing system is configured to track incidents independent from normal tickets</t>
   </si>
 </sst>
 </file>
@@ -4562,10 +4574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4643,7 +4655,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -4656,14 +4668,11 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>376</v>
-      </c>
       <c r="B6" t="s">
-        <v>349</v>
+        <v>408</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
@@ -4674,10 +4683,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>350</v>
+        <v>406</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
@@ -4688,10 +4697,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>351</v>
+        <v>409</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
@@ -4702,10 +4711,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>352</v>
+        <v>410</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
@@ -4715,8 +4724,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>376</v>
+      </c>
       <c r="B10" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
@@ -4730,10 +4742,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
@@ -4744,7 +4756,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
@@ -4758,10 +4770,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
@@ -4772,7 +4784,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
@@ -4786,7 +4798,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
@@ -4800,10 +4812,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
@@ -4814,13 +4826,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>9</v>
@@ -4828,13 +4840,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>9</v>
@@ -4842,13 +4854,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>9</v>
@@ -4856,7 +4868,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>16</v>
@@ -4870,7 +4882,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>16</v>
@@ -4884,13 +4896,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>9</v>
@@ -4898,7 +4910,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>16</v>
@@ -4912,13 +4924,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>9</v>
@@ -4926,30 +4938,27 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>377</v>
-      </c>
       <c r="B26" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>9</v>
@@ -4957,13 +4966,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>9</v>
@@ -4971,13 +4980,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>9</v>
@@ -4985,27 +4994,30 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>367</v>
+        <v>384</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>377</v>
+      </c>
       <c r="B30" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>9</v>
@@ -5013,7 +5025,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>16</v>
@@ -5026,11 +5038,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>378</v>
-      </c>
       <c r="B32" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>16</v>
@@ -5044,7 +5053,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>16</v>
@@ -5058,10 +5067,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>9</v>
@@ -5072,7 +5081,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>16</v>
@@ -5085,14 +5094,17 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>378</v>
+      </c>
       <c r="B36" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>9</v>
@@ -5100,13 +5112,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>395</v>
+        <v>370</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>9</v>
@@ -5114,10 +5126,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>9</v>
@@ -5128,13 +5140,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>9</v>
@@ -5142,7 +5154,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>16</v>
@@ -5156,7 +5168,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>16</v>
@@ -5170,7 +5182,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>399</v>
+        <v>380</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>16</v>
@@ -5183,17 +5195,14 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>394</v>
-      </c>
       <c r="B43" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>9</v>
@@ -5201,13 +5210,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>9</v>
@@ -5215,7 +5224,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>16</v>
@@ -5229,7 +5238,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>16</v>
@@ -5242,8 +5251,11 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>394</v>
+      </c>
       <c r="B47" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>16</v>
@@ -5257,7 +5269,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>16</v>
@@ -5271,7 +5283,7 @@
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>16</v>
@@ -5285,7 +5297,7 @@
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>16</v>
@@ -5299,7 +5311,7 @@
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>16</v>
@@ -5313,7 +5325,7 @@
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>16</v>
@@ -5327,7 +5339,7 @@
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>16</v>
@@ -5341,13 +5353,13 @@
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>9</v>
@@ -5355,13 +5367,13 @@
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>9</v>
@@ -5369,13 +5381,13 @@
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>9</v>
@@ -5383,13 +5395,13 @@
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>9</v>
@@ -5397,15 +5409,71 @@
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>400</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>401</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>402</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>404</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>403</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E58" s="1" t="s">
+      <c r="C62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added threat simulation section, IR playbooks/levers
</commit_message>
<xml_diff>
--- a/Threat-Management-Levels.xlsx
+++ b/Threat-Management-Levels.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="420">
   <si>
     <t>ASVS Item #</t>
   </si>
@@ -1214,9 +1214,6 @@
     <t>Verify incident timeline is being documented</t>
   </si>
   <si>
-    <t>5. Documentation/Metrics</t>
-  </si>
-  <si>
     <t>Verify threat modeling standard exists</t>
   </si>
   <si>
@@ -1272,6 +1269,27 @@
   </si>
   <si>
     <t>Verify mean time to incident resolution is being calculated</t>
+  </si>
+  <si>
+    <t>5. Threat Simulation</t>
+  </si>
+  <si>
+    <t>6. Documentation/Metrics</t>
+  </si>
+  <si>
+    <t>Verify a basic 40 hour penetration test is performed annually</t>
+  </si>
+  <si>
+    <t>Verify a collaborative purple team engagement is performed annually</t>
+  </si>
+  <si>
+    <t>Verify a complex red team test based on threat models and business critical data is performed annually</t>
+  </si>
+  <si>
+    <t>Verify specific incident playbooks exist and are continuously updated</t>
+  </si>
+  <si>
+    <t>Verify Emergency Incident Spend and Lever Execution Standard exists</t>
   </si>
 </sst>
 </file>
@@ -4583,10 +4601,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4650,7 +4668,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
@@ -4664,7 +4682,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -4678,7 +4696,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -4692,7 +4710,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
@@ -4706,7 +4724,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
@@ -4720,7 +4738,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
@@ -4734,7 +4752,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>16</v>
@@ -5141,7 +5159,7 @@
         <v>16</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>9</v>
@@ -5191,7 +5209,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>16</v>
@@ -5225,7 +5243,7 @@
         <v>16</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>9</v>
@@ -5239,7 +5257,7 @@
         <v>16</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>9</v>
@@ -5261,254 +5279,257 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
+        <v>398</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>418</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>419</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>413</v>
+      </c>
+      <c r="B50" t="s">
+        <v>415</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>417</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>416</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>414</v>
+      </c>
+      <c r="B53" t="s">
+        <v>387</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>386</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>393</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>392</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>391</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>390</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>389</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>388</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>395</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>396</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>397</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>399</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>394</v>
-      </c>
-      <c r="B48" t="s">
-        <v>387</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>386</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>393</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>392</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>391</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>390</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>389</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>388</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>396</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>397</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>398</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>400</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>401</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>402</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>404</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>403</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>412</v>
-      </c>
       <c r="C64" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>9</v>
@@ -5516,15 +5537,85 @@
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>401</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>403</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>402</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>411</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>412</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>